<commit_message>
Confirmed cser regression test works
</commit_message>
<xml_diff>
--- a/SampleTestFiles/CSER_Cycles.xlsx
+++ b/SampleTestFiles/CSER_Cycles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BautisSh\source\repos\Personal\WebAutomationTestingProgram\SampleTestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1D0F56-399D-4194-AEDD-56F2AD82F6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C9706E-3191-4198-A082-BFF6B07EF2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,12 +445,6 @@
     <t>K:\ESIP\EDCS QA\QTP\SQL Scripts\CSER\CSER_ReOpen_FANS_Fall24-25.sql</t>
   </si>
   <si>
-    <t>Upload Data File - {Org, Submission}</t>
-  </si>
-  <si>
-    <t>Validate Data File - {Org, Submission}</t>
-  </si>
-  <si>
     <t>Data Submission - {Org, Submission}</t>
   </si>
   <si>
@@ -461,6 +455,12 @@
   </si>
   <si>
     <t>Upload Letter - {Org, Submission}</t>
+  </si>
+  <si>
+    <t>Step 1 Upload Data File - {Org, Submission}</t>
+  </si>
+  <si>
+    <t>Step 2 Validate Data File - {Org, Submission}</t>
   </si>
 </sst>
 </file>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
         <v>103</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>42</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>48</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>51</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="16" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>102</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>55</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>30</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>56</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>36</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>42</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="22" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>57</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>59</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>51</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>54</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>55</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>30</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>56</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>42</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="32" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>61</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>63</v>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>51</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>54</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>55</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>30</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>56</v>
@@ -2668,7 +2668,7 @@
     </row>
     <row r="43" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>36</v>
@@ -2712,7 +2712,7 @@
     </row>
     <row r="44" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>42</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>71</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>59</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>51</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>54</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>55</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>30</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>56</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>36</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="57" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>42</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="58" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>74</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>76</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>51</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="61" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>54</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>55</v>
@@ -3503,7 +3503,7 @@
     </row>
     <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>30</v>
@@ -3547,7 +3547,7 @@
     </row>
     <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>56</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>36</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>42</v>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>79</v>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="68" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>45</v>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="69" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>82</v>
@@ -3811,7 +3811,7 @@
     </row>
     <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>51</v>
@@ -3869,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A481E-4312-4BB7-973A-96CD3C5B6711}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>